<commit_message>
station_name_change updated, applied changes to transect.locations
</commit_message>
<xml_diff>
--- a/Oyster_data/Transect/station_name_change.xlsx
+++ b/Oyster_data/Transect/station_name_change.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Oyster Project\project_task\t3_precon_mon\oyster\map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevenbeck\Desktop\Reef_Project\Git\Data\oyster_data\transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="134">
   <si>
     <t>Epoch</t>
   </si>
@@ -403,6 +403,24 @@
   </si>
   <si>
     <t>rock</t>
+  </si>
+  <si>
+    <t>LCN9</t>
+  </si>
+  <si>
+    <t>CRO4</t>
+  </si>
+  <si>
+    <t>HBN5</t>
+  </si>
+  <si>
+    <t>HBN6</t>
+  </si>
+  <si>
+    <t>Appears only 12/8/2010 sample was mislabeled</t>
+  </si>
+  <si>
+    <t>7/7/2010 sample correct</t>
   </si>
 </sst>
 </file>
@@ -1217,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,25 +1365,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5">
-        <v>306120</v>
+        <v>305815</v>
       </c>
       <c r="G5">
-        <v>3227868</v>
+        <v>3227137</v>
       </c>
       <c r="H5" t="s">
         <v>126</v>
@@ -1385,16 +1403,16 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6">
-        <v>306158</v>
+        <v>306120</v>
       </c>
       <c r="G6">
-        <v>3227983</v>
+        <v>3227868</v>
       </c>
       <c r="H6" t="s">
         <v>126</v>
@@ -1414,16 +1432,16 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7">
-        <v>306646</v>
+        <v>306158</v>
       </c>
       <c r="G7">
-        <v>3228017</v>
+        <v>3227983</v>
       </c>
       <c r="H7" t="s">
         <v>126</v>
@@ -1437,22 +1455,22 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8">
-        <v>306778</v>
+        <v>306646</v>
       </c>
       <c r="G8">
-        <v>3228724</v>
+        <v>3228017</v>
       </c>
       <c r="H8" t="s">
         <v>126</v>
@@ -1472,16 +1490,16 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
       <c r="F9">
-        <v>306883</v>
+        <v>306778</v>
       </c>
       <c r="G9">
-        <v>3228814</v>
+        <v>3228724</v>
       </c>
       <c r="H9" t="s">
         <v>126</v>
@@ -1501,16 +1519,16 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10">
-        <v>306723</v>
+        <v>306883</v>
       </c>
       <c r="G10">
-        <v>3228950</v>
+        <v>3228814</v>
       </c>
       <c r="H10" t="s">
         <v>126</v>
@@ -1524,22 +1542,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>298326</v>
+        <v>306723</v>
       </c>
       <c r="G11">
-        <v>3226099</v>
+        <v>3228950</v>
       </c>
       <c r="H11" t="s">
         <v>126</v>
@@ -1559,16 +1577,16 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12">
-        <v>298351</v>
+        <v>298326</v>
       </c>
       <c r="G12">
-        <v>3225980</v>
+        <v>3226099</v>
       </c>
       <c r="H12" t="s">
         <v>126</v>
@@ -1588,16 +1606,16 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13">
-        <v>298392</v>
+        <v>298351</v>
       </c>
       <c r="G13">
-        <v>3226055</v>
+        <v>3225980</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -1611,22 +1629,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14">
-        <v>299767</v>
+        <v>298392</v>
       </c>
       <c r="G14">
-        <v>3227182</v>
+        <v>3226055</v>
       </c>
       <c r="H14" t="s">
         <v>126</v>
@@ -1646,16 +1664,16 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15">
-        <v>299777</v>
+        <v>299767</v>
       </c>
       <c r="G15">
-        <v>3226660</v>
+        <v>3227182</v>
       </c>
       <c r="H15" t="s">
         <v>126</v>
@@ -1675,16 +1693,16 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16">
-        <v>299555</v>
+        <v>299777</v>
       </c>
       <c r="G16">
-        <v>3227068</v>
+        <v>3226660</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -1698,22 +1716,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17">
-        <v>300804</v>
+        <v>299555</v>
       </c>
       <c r="G17">
-        <v>3227972</v>
+        <v>3227068</v>
       </c>
       <c r="H17" t="s">
         <v>126</v>
@@ -1733,16 +1751,16 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18">
-        <v>300736</v>
+        <v>300804</v>
       </c>
       <c r="G18">
-        <v>3227813</v>
+        <v>3227972</v>
       </c>
       <c r="H18" t="s">
         <v>126</v>
@@ -1762,16 +1780,16 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
       </c>
       <c r="F19">
-        <v>300734</v>
+        <v>300736</v>
       </c>
       <c r="G19">
-        <v>3228267</v>
+        <v>3227813</v>
       </c>
       <c r="H19" t="s">
         <v>126</v>
@@ -1785,28 +1803,28 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
       </c>
       <c r="F20">
-        <v>282938</v>
+        <v>300734</v>
       </c>
       <c r="G20">
-        <v>3254310</v>
+        <v>3228267</v>
       </c>
       <c r="H20" t="s">
         <v>126</v>
       </c>
       <c r="I20" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1820,16 +1838,16 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
       </c>
       <c r="F21">
-        <v>282263</v>
+        <v>282938</v>
       </c>
       <c r="G21">
-        <v>3254820</v>
+        <v>3254310</v>
       </c>
       <c r="H21" t="s">
         <v>126</v>
@@ -1849,16 +1867,16 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
       </c>
       <c r="F22">
-        <v>280813</v>
+        <v>282263</v>
       </c>
       <c r="G22">
-        <v>3256105</v>
+        <v>3254820</v>
       </c>
       <c r="H22" t="s">
         <v>126</v>
@@ -1872,22 +1890,22 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
         <v>9</v>
       </c>
       <c r="F23">
-        <v>284468</v>
+        <v>280813</v>
       </c>
       <c r="G23">
-        <v>3255825</v>
+        <v>3256105</v>
       </c>
       <c r="H23" t="s">
         <v>126</v>
@@ -1907,16 +1925,16 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="F24">
-        <v>283586</v>
+        <v>284468</v>
       </c>
       <c r="G24">
-        <v>3256287</v>
+        <v>3255825</v>
       </c>
       <c r="H24" t="s">
         <v>126</v>
@@ -1936,16 +1954,16 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
       </c>
       <c r="F25">
-        <v>283203</v>
+        <v>283586</v>
       </c>
       <c r="G25">
-        <v>3256270</v>
+        <v>3256287</v>
       </c>
       <c r="H25" t="s">
         <v>126</v>
@@ -1959,22 +1977,22 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
       </c>
       <c r="F26">
-        <v>284203</v>
+        <v>283203</v>
       </c>
       <c r="G26">
-        <v>3257040</v>
+        <v>3256270</v>
       </c>
       <c r="H26" t="s">
         <v>126</v>
@@ -1988,57 +2006,57 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
       </c>
       <c r="F27">
-        <v>285242</v>
+        <v>280659</v>
       </c>
       <c r="G27">
-        <v>3256430</v>
+        <v>3257379</v>
       </c>
       <c r="H27" t="s">
         <v>126</v>
       </c>
       <c r="I27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28">
-        <v>284311</v>
-      </c>
-      <c r="G28">
-        <v>3256902</v>
-      </c>
-      <c r="H28" t="s">
-        <v>126</v>
-      </c>
-      <c r="I28" t="s">
-        <v>36</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="1">
+        <v>283641</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3256262</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2046,22 +2064,22 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
       </c>
       <c r="F29">
-        <v>284067</v>
+        <v>280182</v>
       </c>
       <c r="G29">
-        <v>3256766</v>
+        <v>3257594</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -2070,91 +2088,91 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="1">
-        <v>294865</v>
-      </c>
-      <c r="G30" s="1">
-        <v>3238692</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="1">
-        <v>294686</v>
-      </c>
-      <c r="G31" s="1">
-        <v>3238948</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F32" s="1">
-        <v>294395</v>
-      </c>
-      <c r="G32" s="1">
-        <v>3239164</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>11</v>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30">
+        <v>284203</v>
+      </c>
+      <c r="G30">
+        <v>3257040</v>
+      </c>
+      <c r="H30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>285242</v>
+      </c>
+      <c r="G31">
+        <v>3256430</v>
+      </c>
+      <c r="H31" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32">
+        <v>284311</v>
+      </c>
+      <c r="G32">
+        <v>3256902</v>
+      </c>
+      <c r="H32" t="s">
+        <v>126</v>
+      </c>
+      <c r="I32" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2162,56 +2180,56 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
       </c>
       <c r="F33">
-        <v>298380</v>
+        <v>284067</v>
       </c>
       <c r="G33">
-        <v>3236557</v>
+        <v>3256766</v>
       </c>
       <c r="H33" t="s">
         <v>126</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34">
-        <v>298651</v>
-      </c>
-      <c r="G34">
-        <v>3236638</v>
-      </c>
-      <c r="H34" t="s">
-        <v>126</v>
-      </c>
-      <c r="I34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="1">
+        <v>294865</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3238692</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2220,22 +2238,22 @@
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F35" s="1">
-        <v>297907</v>
+        <v>294686</v>
       </c>
       <c r="G35" s="1">
-        <v>3234553</v>
+        <v>3238948</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>126</v>
@@ -2249,22 +2267,22 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F36" s="1">
-        <v>298534</v>
+        <v>294395</v>
       </c>
       <c r="G36" s="1">
-        <v>3236727</v>
+        <v>3239164</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>126</v>
@@ -2278,22 +2296,22 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
       </c>
       <c r="F37">
-        <v>299282</v>
+        <v>298380</v>
       </c>
       <c r="G37">
-        <v>3235919</v>
+        <v>3236557</v>
       </c>
       <c r="H37" t="s">
         <v>126</v>
@@ -2307,22 +2325,22 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
       </c>
       <c r="F38">
-        <v>298841</v>
+        <v>298651</v>
       </c>
       <c r="G38">
-        <v>3235773</v>
+        <v>3236638</v>
       </c>
       <c r="H38" t="s">
         <v>126</v>
@@ -2331,178 +2349,178 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="1">
+        <v>297907</v>
+      </c>
+      <c r="G39" s="1">
+        <v>3234553</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="1">
+        <v>298534</v>
+      </c>
+      <c r="G40" s="1">
+        <v>3236727</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" s="1">
+        <v>297281</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3233308</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>61</v>
       </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42">
+        <v>299282</v>
+      </c>
+      <c r="G42">
+        <v>3235919</v>
+      </c>
+      <c r="H42" t="s">
+        <v>126</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43">
+        <v>298841</v>
+      </c>
+      <c r="G43">
+        <v>3235773</v>
+      </c>
+      <c r="H43" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
         <v>64</v>
       </c>
-      <c r="E39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39">
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44">
         <v>298763</v>
       </c>
-      <c r="G39">
+      <c r="G44">
         <v>3235642</v>
       </c>
-      <c r="H39" t="s">
-        <v>126</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="H44" t="s">
+        <v>126</v>
+      </c>
+      <c r="I44" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" s="1">
-        <v>294705.8677</v>
-      </c>
-      <c r="G40" s="1">
-        <v>3238859.4249999998</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F41" s="1">
-        <v>294806.66590000002</v>
-      </c>
-      <c r="G41" s="1">
-        <v>3238782.88</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" s="1">
-        <v>294931.07270000002</v>
-      </c>
-      <c r="G42" s="1">
-        <v>3238656.7960000001</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="1">
-        <v>295040.48879999999</v>
-      </c>
-      <c r="G43" s="1">
-        <v>3238583.5350000001</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F44" s="1">
-        <v>295141.48430000001</v>
-      </c>
-      <c r="G44" s="1">
-        <v>3238469.0720000002</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2510,22 +2528,22 @@
         <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F45" s="1">
-        <v>295253.55729999999</v>
+        <v>294705.8677</v>
       </c>
       <c r="G45" s="1">
-        <v>3238278.4649999999</v>
+        <v>3238859.4249999998</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>127</v>
@@ -2539,25 +2557,25 @@
         <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F46" s="1">
-        <v>295308.54570000002</v>
+        <v>294806.66590000002</v>
       </c>
       <c r="G46" s="1">
-        <v>3238216.719</v>
+        <v>3238782.88</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>68</v>
@@ -2568,22 +2586,22 @@
         <v>65</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="F47" s="1">
-        <v>295423.44420000003</v>
+        <v>294931.07270000002</v>
       </c>
       <c r="G47" s="1">
-        <v>3238074.8459999999</v>
+        <v>3238656.7960000001</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>126</v>
@@ -2592,149 +2610,149 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>3</v>
-      </c>
-      <c r="B48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48">
-        <v>297465.30910000001</v>
-      </c>
-      <c r="G48">
-        <v>3239361.4619999998</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
-        <v>91</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49">
-        <v>297612.75189999997</v>
-      </c>
-      <c r="G49">
-        <v>3239507.4040000001</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>3</v>
-      </c>
-      <c r="B50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50">
-        <v>297677.8958</v>
-      </c>
-      <c r="G50">
-        <v>3239398.7030000002</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I50" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>3</v>
-      </c>
-      <c r="B51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s">
-        <v>95</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51">
-        <v>297601.96059999999</v>
-      </c>
-      <c r="G51">
-        <v>3239173.8790000002</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>3</v>
-      </c>
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s">
-        <v>98</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52">
-        <v>298243.08319999999</v>
-      </c>
-      <c r="G52">
-        <v>3238323.22</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I52" t="s">
-        <v>99</v>
+    <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" s="1">
+        <v>295040.48879999999</v>
+      </c>
+      <c r="G48" s="1">
+        <v>3238583.5350000001</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="1">
+        <v>295141.48430000001</v>
+      </c>
+      <c r="G49" s="1">
+        <v>3238469.0720000002</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="1">
+        <v>295253.55729999999</v>
+      </c>
+      <c r="G50" s="1">
+        <v>3238278.4649999999</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F51" s="1">
+        <v>295308.54570000002</v>
+      </c>
+      <c r="G51" s="1">
+        <v>3238216.719</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" s="1">
+        <v>295423.44420000003</v>
+      </c>
+      <c r="G52" s="1">
+        <v>3238074.8459999999</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2742,28 +2760,28 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E53" t="s">
         <v>9</v>
       </c>
       <c r="F53">
-        <v>298243.08319999999</v>
+        <v>297465.30910000001</v>
       </c>
       <c r="G53">
-        <v>3238323.22</v>
+        <v>3239361.4619999998</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>126</v>
       </c>
       <c r="I53" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2771,28 +2789,28 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E54" t="s">
         <v>9</v>
       </c>
       <c r="F54">
-        <v>298339.76329999999</v>
+        <v>297612.75189999997</v>
       </c>
       <c r="G54">
-        <v>3238402.4419999998</v>
+        <v>3239507.4040000001</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>126</v>
       </c>
       <c r="I54" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2800,28 +2818,28 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C55" t="s">
         <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
         <v>9</v>
       </c>
       <c r="F55">
-        <v>298294.24099999998</v>
+        <v>297677.8958</v>
       </c>
       <c r="G55">
-        <v>3238521.878</v>
+        <v>3239398.7030000002</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>126</v>
       </c>
       <c r="I55" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2829,28 +2847,28 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E56" t="s">
         <v>9</v>
       </c>
       <c r="F56">
-        <v>298530.71789999999</v>
+        <v>297601.96059999999</v>
       </c>
       <c r="G56">
-        <v>3237216.0950000002</v>
+        <v>3239173.8790000002</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>126</v>
       </c>
       <c r="I56" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2858,173 +2876,173 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57">
+        <v>298243.08319999999</v>
+      </c>
+      <c r="G57">
+        <v>3238323.22</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I57" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>298243.08319999999</v>
+      </c>
+      <c r="G58">
+        <v>3238323.22</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>298339.76329999999</v>
+      </c>
+      <c r="G59">
+        <v>3238402.4419999998</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>104</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <v>298294.24099999998</v>
+      </c>
+      <c r="G60">
+        <v>3238521.878</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
         <v>106</v>
       </c>
-      <c r="C57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61">
+        <v>298530.71789999999</v>
+      </c>
+      <c r="G61">
+        <v>3237216.0950000002</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
         <v>109</v>
       </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57">
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62">
         <v>298480.19150000002</v>
       </c>
-      <c r="G57">
+      <c r="G62">
         <v>3237712.571</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I57" t="s">
+      <c r="H62" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I62" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>3</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F58" s="1">
-        <v>294376.62640000001</v>
-      </c>
-      <c r="G58" s="1">
-        <v>3239243.8829999999</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>3</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F59" s="1">
-        <v>294488.02289999998</v>
-      </c>
-      <c r="G59" s="1">
-        <v>3239060.0419999999</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>3</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F60" s="1">
-        <v>294488.02289999998</v>
-      </c>
-      <c r="G60" s="1">
-        <v>3239060.0419999999</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>3</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F61" s="1">
-        <v>298820.98680000001</v>
-      </c>
-      <c r="G61" s="1">
-        <v>3236639.9939999999</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>3</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F62" s="1">
-        <v>298807.66529999999</v>
-      </c>
-      <c r="G62" s="1">
-        <v>3236766.6189999999</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3032,22 +3050,22 @@
         <v>3</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="F63" s="1">
-        <v>298317.16769999999</v>
+        <v>294376.62640000001</v>
       </c>
       <c r="G63" s="1">
-        <v>3235753.085</v>
+        <v>3239243.8829999999</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>126</v>
@@ -3061,22 +3079,22 @@
         <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="F64" s="1">
-        <v>298713.97230000002</v>
+        <v>294488.02289999998</v>
       </c>
       <c r="G64" s="1">
-        <v>3235921.2409999999</v>
+        <v>3239060.0419999999</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>126</v>
@@ -3090,22 +3108,22 @@
         <v>3</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F65" s="1">
-        <v>298843.6606</v>
+        <v>294488.02289999998</v>
       </c>
       <c r="G65" s="1">
-        <v>3235996.5589999999</v>
+        <v>3239060.0419999999</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>126</v>
@@ -3119,27 +3137,172 @@
         <v>3</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F66" s="1">
+        <v>298820.98680000001</v>
+      </c>
+      <c r="G66" s="1">
+        <v>3236639.9939999999</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>3</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" s="1">
+        <v>298807.66529999999</v>
+      </c>
+      <c r="G67" s="1">
+        <v>3236766.6189999999</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>3</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" s="1" t="s">
+      <c r="C68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F68" s="1">
+        <v>298317.16769999999</v>
+      </c>
+      <c r="G68" s="1">
+        <v>3235753.085</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>3</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F69" s="1">
+        <v>298713.97230000002</v>
+      </c>
+      <c r="G69" s="1">
+        <v>3235921.2409999999</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>3</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F70" s="1">
+        <v>298843.6606</v>
+      </c>
+      <c r="G70" s="1">
+        <v>3235996.5589999999</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>3</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F71" s="1">
         <v>298759.4535</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G71" s="1">
         <v>3235633.29</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I66" s="1" t="s">
+      <c r="H71" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>